<commit_message>
updated the testing framework
</commit_message>
<xml_diff>
--- a/documentation/MS2_Testing.xlsx
+++ b/documentation/MS2_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jobroomfield/Desktop/Kids In Tow Project/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28F565-E5F0-D24F-B4D6-644FF92AC5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656DF977-E85D-F244-8AA8-951CC34D02AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{FE313CD3-8A40-1448-A5DF-91EC0D360A9F}"/>
   </bookViews>
@@ -205,9 +205,6 @@
     <t>Search for places of interest on the interactive map</t>
   </si>
   <si>
-    <t xml:space="preserve">When the users selects a place of interest from the dropdown list, when the 'Search' button is clicked, the </t>
-  </si>
-  <si>
     <t>Click on the Contact tab</t>
   </si>
   <si>
@@ -292,7 +289,10 @@
     <t>View content in info window for all places</t>
   </si>
   <si>
-    <t>When the user clicks on a marker, an info window pops out revealing the placew name, address, rating and link to the website</t>
+    <t>When the users selects a place of interest from the dropdown list, when the 'Search' button is clicked, the results are displayed on the map as a series of markers. Markers are different depending on the 'type' selected by the user.</t>
+  </si>
+  <si>
+    <t>When the user clicks on a marker, an info window pops out revealing the place name, address, rating and link to the website</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E48B459-AC57-764F-8C01-E5DD33D8F3AE}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,10 +1035,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
@@ -1073,10 +1073,10 @@
         <v>28</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>0</v>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>0</v>
@@ -1161,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>0</v>
@@ -1395,10 +1395,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>0</v>
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -1453,10 +1453,10 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>0</v>
@@ -1491,10 +1491,10 @@
         <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>0</v>
@@ -1547,10 +1547,10 @@
         <v>0</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>0</v>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>0</v>
@@ -1623,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>86</v>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>0</v>
@@ -1716,13 +1716,13 @@
     </row>
     <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>0</v>
@@ -1754,13 +1754,13 @@
     </row>
     <row r="24" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>0</v>
@@ -1792,13 +1792,13 @@
     </row>
     <row r="25" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>0</v>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>0</v>
@@ -1830,13 +1830,13 @@
     </row>
     <row r="26" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>0</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="27" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>0</v>
@@ -1906,13 +1906,13 @@
     </row>
     <row r="28" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>0</v>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>0</v>
@@ -1944,13 +1944,13 @@
     </row>
     <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>0</v>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>0</v>

</xml_diff>